<commit_message>
Dec 02 Signed-off-by: cyrexxx <kartik@kth.se>
</commit_message>
<xml_diff>
--- a/MPPT_i_voc.xlsx
+++ b/MPPT_i_voc.xlsx
@@ -562,7 +562,7 @@
                   <c:v>3.372456344081904</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.372456344081904</c:v>
+                  <c:v>3.3724563440819</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>3.3908843203999393</c:v>
@@ -745,11 +745,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153684992"/>
-        <c:axId val="153719552"/>
+        <c:axId val="224463872"/>
+        <c:axId val="224490240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153684992"/>
+        <c:axId val="224463872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,12 +759,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153719552"/>
+        <c:crossAx val="224490240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153719552"/>
+        <c:axId val="224490240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153684992"/>
+        <c:crossAx val="224463872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1552,11 +1552,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153960832"/>
-        <c:axId val="153962368"/>
+        <c:axId val="224743808"/>
+        <c:axId val="224745344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153960832"/>
+        <c:axId val="224743808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,12 +1566,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153962368"/>
+        <c:crossAx val="224745344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153962368"/>
+        <c:axId val="224745344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153960832"/>
+        <c:crossAx val="224743808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2272,11 +2272,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153991424"/>
-        <c:axId val="153993216"/>
+        <c:axId val="224778496"/>
+        <c:axId val="224780288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153991424"/>
+        <c:axId val="224778496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2286,12 +2286,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153993216"/>
+        <c:crossAx val="224780288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153993216"/>
+        <c:axId val="224780288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,7 +2302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153991424"/>
+        <c:crossAx val="224778496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2742,10 +2742,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:J100"/>
+  <dimension ref="D1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="AD71" sqref="AD71"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="X49" sqref="X49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3288,7 +3288,7 @@
         <v>3.2824563440819041</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D33">
         <v>3.1714483242355347</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>3.2824563440819041</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D34">
         <v>3.279436534228922</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>3.2824563440819041</v>
       </c>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D35">
         <v>3.3875571253657699</v>
       </c>
@@ -3339,7 +3339,7 @@
         <v>3.3107397276287776</v>
       </c>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D36">
         <v>3.4956806243211447</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>3.3508071672478197</v>
       </c>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D37">
         <v>3.6036775577700522</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>3.3532975791608317</v>
       </c>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D38">
         <v>3.7114184523875529</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>3.3563847724236529</v>
       </c>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D39">
         <v>3.8187738348487228</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>3.3721788014978249</v>
       </c>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D40">
         <v>3.9285471106603054</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>3.372456344081904</v>
       </c>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D41">
         <v>4.0378130600291486</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>3.372456344081904</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D42">
         <v>4.146193063926086</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>3.372456344081904</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D43">
         <v>4.2538302048265617</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>3.372456344081904</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D44">
         <v>4.3609256222589314</v>
       </c>
@@ -3489,10 +3489,10 @@
         <v>1.2931006890308976</v>
       </c>
       <c r="J44">
-        <v>3.372456344081904</v>
-      </c>
-    </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.3">
+        <v>3.3724563440819</v>
+      </c>
+    </row>
+    <row r="45" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D45">
         <v>4.4676804557515633</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>3.3908843203999393</v>
       </c>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D46">
         <v>4.5742958448327808</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>3.3933102522947527</v>
       </c>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D47">
         <v>4.6809729290309576</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>3.3967398215414635</v>
       </c>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D48">
         <v>4.7879128478744821</v>
       </c>
@@ -3559,8 +3559,11 @@
       <c r="J48">
         <v>3.410690492306657</v>
       </c>
-    </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="X48">
+        <v>3.9630000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D49">
         <v>4.8953167408916327</v>
       </c>
@@ -3576,8 +3579,12 @@
       <c r="J49">
         <v>3.4118402769093543</v>
       </c>
-    </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="X49">
+        <f>(0.9586*X48)-0.5409</f>
+        <v>3.2580317999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D50">
         <v>5.0033857476107952</v>
       </c>
@@ -3594,7 +3601,7 @@
         <v>3.4127280909213566</v>
       </c>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D51">
         <v>5.1123210075603618</v>
       </c>
@@ -3611,7 +3618,7 @@
         <v>3.4133800643119003</v>
       </c>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>5.2223886668118906</v>
       </c>
@@ -3628,7 +3635,7 @@
         <v>3.413805168234024</v>
       </c>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D53">
         <v>5.3335348720733702</v>
       </c>
@@ -3645,7 +3652,7 @@
         <v>3.4140703676183151</v>
       </c>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D54">
         <v>5.4454807638277885</v>
       </c>
@@ -3662,7 +3669,7 @@
         <v>3.4142416219541953</v>
       </c>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D55">
         <v>5.5579474825580322</v>
       </c>
@@ -3679,7 +3686,7 @@
         <v>3.4423212184209442</v>
       </c>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D56">
         <v>5.6706561687470325</v>
       </c>
@@ -3696,7 +3703,7 @@
         <v>3.4619006968189852</v>
       </c>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D57">
         <v>5.7862689185063996</v>
       </c>
@@ -3713,7 +3720,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D58">
         <v>5.901852235834502</v>
       </c>
@@ -3730,7 +3737,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="59" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D59">
         <v>6.0168244126933477</v>
       </c>
@@ -3747,7 +3754,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D60">
         <v>6.1309024208376899</v>
       </c>
@@ -3764,7 +3771,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="61" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D61">
         <v>6.2438032320222838</v>
       </c>
@@ -3781,7 +3788,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="62" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D62">
         <v>6.3555907005475971</v>
       </c>
@@ -3798,7 +3805,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="63" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D63">
         <v>6.4668801798769229</v>
       </c>
@@ -3815,7 +3822,7 @@
         <v>3.4624563440819038</v>
       </c>
     </row>
-    <row r="64" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D64">
         <v>6.5777468346678658</v>
       </c>

</xml_diff>